<commit_message>
Update TABELA DE PUBLICIDADE.xlsx
</commit_message>
<xml_diff>
--- a/TABELA DE PUBLICIDADE.xlsx
+++ b/TABELA DE PUBLICIDADE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ipsetubal-my.sharepoint.com/personal/202100275_estudantes_ips_pt/Documents/Ambiente de Trabalho/Personal/DINU/Calculadora Publicidade/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ipsetubal-my.sharepoint.com/personal/202100275_estudantes_ips_pt/Documents/Ambiente de Trabalho/Personal/DINU/calculadora-unife/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{52AA7B78-9435-4DD8-BE93-F8B18B06835E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9274E9E6-5323-4EB2-B63E-7C1061231437}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{52AA7B78-9435-4DD8-BE93-F8B18B06835E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBF3F088-DA26-4714-98C5-D0ADDF7054DA}"/>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="3555" windowWidth="21630" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5025" yWindow="3225" windowWidth="21630" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Price" sheetId="2" r:id="rId1"/>
@@ -92,9 +92,6 @@
     <t>18:00 - 20:00</t>
   </si>
   <si>
-    <t>20:00 - 25:00</t>
-  </si>
-  <si>
     <t>FIM DE SEMANA</t>
   </si>
   <si>
@@ -108,6 +105,9 @@
   </si>
   <si>
     <t>Comissão(%)</t>
+  </si>
+  <si>
+    <t>20:00 - 01:00</t>
   </si>
 </sst>
 </file>
@@ -472,7 +472,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -729,7 +729,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B7" s="4">
         <v>421.42</v>
@@ -770,7 +770,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>1</v>
@@ -811,7 +811,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="4">
         <v>90.45</v>
@@ -1016,7 +1016,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="4">
         <v>390.42</v>
@@ -1057,7 +1057,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1065,7 +1065,7 @@
         <v>10</v>
       </c>
       <c r="I18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>